<commit_message>
Atualização dos dados [Detalhe da atualização, ex: semanal, mensal, novas visitas]
</commit_message>
<xml_diff>
--- a/dClientes.xlsx
+++ b/dClientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fatbr\Desktop\Estrutura Equipe NWB_2025\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED7C9FC2-83E4-44EB-A5C4-03F59B56D161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2B60EB-4AD2-4728-964E-7E94708A5B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{8CEE68A8-301B-4019-BF26-44DB06A18B9F}"/>
   </bookViews>
@@ -4602,7 +4602,9 @@
   </sheetPr>
   <dimension ref="A1:AX163"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.25"/>
   <cols>

</xml_diff>